<commit_message>
wip... 231112piu_a - ALMOST READY - to analyze results, clean and prep nxt actions
</commit_message>
<xml_diff>
--- a/base_proc/test_data_and_specs/test_fact_RENware/fact_RENF1004.xlsx
+++ b/base_proc/test_data_and_specs/test_fact_RENware/fact_RENF1004.xlsx
@@ -525,7 +525,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -670,10 +670,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="18" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -732,10 +728,6 @@
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="16" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -765,24 +757,24 @@
   </sheetPr>
   <dimension ref="A2:M37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="1.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="1.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="1.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="1.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="3.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="1.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="3.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="1.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="1.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1000" min="14" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="1.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1000" min="14" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1001" style="0" width="11.43"/>
   </cols>
   <sheetData>
@@ -1098,344 +1090,344 @@
         <f aca="false">3000*4.9358</f>
         <v>14807.4</v>
       </c>
-      <c r="K17" s="36" t="n">
+      <c r="K17" s="35" t="n">
         <f aca="false">ROUND(J17*H17,2)</f>
         <v>14807.4</v>
       </c>
-      <c r="L17" s="37" t="n">
+      <c r="L17" s="36" t="n">
         <f aca="false">ROUND(K17*19%, 2)</f>
         <v>2813.41</v>
       </c>
-      <c r="M17" s="37"/>
+      <c r="M17" s="36"/>
     </row>
     <row r="18" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39" t="s">
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
     </row>
     <row r="19" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="39" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
     </row>
     <row r="20" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39" t="s">
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
     </row>
     <row r="21" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
     </row>
     <row r="22" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
     </row>
     <row r="23" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
     </row>
     <row r="24" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
     </row>
     <row r="25" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="38"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
     </row>
     <row r="26" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
     </row>
     <row r="27" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="38"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
     </row>
     <row r="28" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
     </row>
     <row r="29" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
     </row>
     <row r="30" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="38"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41"/>
     </row>
     <row r="31" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="38"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="45" t="s">
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="46" t="s">
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="47" t="n">
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="46" t="n">
         <f aca="false">SUM(K17:K31)</f>
         <v>14807.4</v>
       </c>
-      <c r="L32" s="48" t="n">
+      <c r="L32" s="47" t="n">
         <f aca="false">SUM(L17:M31)</f>
         <v>2813.41</v>
       </c>
-      <c r="M32" s="48"/>
+      <c r="M32" s="47"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="49" t="s">
+      <c r="A33" s="43"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="50" t="s">
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="51" t="n">
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="50" t="n">
         <f aca="false">K32+L32</f>
         <v>17620.81</v>
       </c>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="50"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="44"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="52" t="s">
+      <c r="A34" s="43"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="50"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="44"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="53" t="s">
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="44"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="53"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="44"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="112">

</xml_diff>